<commit_message>
Excel file now has headers centered automatically and the font they possess is bolded
</commit_message>
<xml_diff>
--- a/Power_League_Stats.xlsx
+++ b/Power_League_Stats.xlsx
@@ -2,27 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="400" yWindow="520" windowWidth="27640" windowHeight="15080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Power League Stats" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="12"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
@@ -47,12 +52,14 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -135,44 +142,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -199,32 +206,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -251,24 +240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -280,142 +251,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -425,2982 +420,2837 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A904:D1185"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col width="10.83203125" customWidth="1" style="1" min="2" max="2"/>
-    <col width="16.5" bestFit="1" customWidth="1" min="3" max="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="904"/>
-    <row r="905"/>
-    <row r="906"/>
-    <row r="907"/>
-    <row r="908"/>
-    <row r="909"/>
-    <row r="910"/>
-    <row r="911"/>
-    <row r="912"/>
-    <row r="913"/>
-    <row r="914"/>
-    <row r="915"/>
-    <row r="916"/>
-    <row r="917"/>
-    <row r="918"/>
-    <row r="919"/>
-    <row r="920"/>
-    <row r="921"/>
-    <row r="922"/>
-    <row r="923"/>
-    <row r="924"/>
-    <row r="925"/>
-    <row r="926"/>
-    <row r="927"/>
-    <row r="928"/>
-    <row r="929"/>
-    <row r="930"/>
-    <row r="931"/>
-    <row r="932"/>
-    <row r="933"/>
-    <row r="934"/>
-    <row r="935"/>
-    <row r="936"/>
-    <row r="937"/>
-    <row r="938"/>
-    <row r="939"/>
-    <row r="940"/>
-    <row r="941"/>
-    <row r="942"/>
-    <row r="943"/>
-    <row r="944"/>
-    <row r="945"/>
-    <row r="946"/>
-    <row r="947"/>
-    <row r="948"/>
-    <row r="949"/>
-    <row r="950"/>
-    <row r="951"/>
-    <row r="952"/>
-    <row r="953"/>
-    <row r="954"/>
-    <row r="955"/>
-    <row r="956"/>
-    <row r="957"/>
-    <row r="958"/>
-    <row r="959"/>
-    <row r="960"/>
-    <row r="961"/>
-    <row r="962"/>
-    <row r="963"/>
-    <row r="964"/>
-    <row r="965"/>
-    <row r="966"/>
-    <row r="967"/>
-    <row r="968"/>
-    <row r="969"/>
-    <row r="970"/>
-    <row r="971"/>
-    <row r="972"/>
-    <row r="973"/>
-    <row r="974"/>
-    <row r="975"/>
-    <row r="976"/>
-    <row r="977"/>
-    <row r="978"/>
-    <row r="979"/>
-    <row r="980"/>
-    <row r="981"/>
-    <row r="982"/>
-    <row r="983"/>
-    <row r="984"/>
-    <row r="985"/>
-    <row r="986"/>
-    <row r="987"/>
-    <row r="988"/>
-    <row r="989"/>
-    <row r="990"/>
-    <row r="991"/>
-    <row r="992"/>
-    <row r="993"/>
-    <row r="994"/>
-    <row r="995"/>
-    <row r="996"/>
-    <row r="997"/>
-    <row r="998"/>
-    <row r="999"/>
-    <row r="1000"/>
-    <row r="1001"/>
-    <row r="1002"/>
-    <row r="1003"/>
-    <row r="1004"/>
-    <row r="1005"/>
-    <row r="1006"/>
-    <row r="1007"/>
-    <row r="1008"/>
-    <row r="1009"/>
-    <row r="1010"/>
-    <row r="1011"/>
-    <row r="1012"/>
-    <row r="1013"/>
-    <row r="1014"/>
-    <row r="1015"/>
-    <row r="1016"/>
-    <row r="1017"/>
-    <row r="1018"/>
-    <row r="1019"/>
-    <row r="1020"/>
-    <row r="1021"/>
-    <row r="1022"/>
-    <row r="1023"/>
-    <row r="1024"/>
-    <row r="1025"/>
-    <row r="1026"/>
-    <row r="1027"/>
-    <row r="1028"/>
-    <row r="1029"/>
-    <row r="1030"/>
-    <row r="1031"/>
-    <row r="1032"/>
-    <row r="1033"/>
-    <row r="1034"/>
-    <row r="1035"/>
-    <row r="1036"/>
-    <row r="1037"/>
-    <row r="1038"/>
-    <row r="1039"/>
-    <row r="1040"/>
-    <row r="1041"/>
-    <row r="1042"/>
-    <row r="1043"/>
-    <row r="1044"/>
-    <row r="1045">
-      <c r="A1045" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Brawler</t>
         </is>
       </c>
-      <c r="B1045" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Win Rate</t>
         </is>
       </c>
-      <c r="C1045" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Map</t>
         </is>
       </c>
-      <c r="D1045" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Map Type</t>
         </is>
       </c>
     </row>
-    <row r="1046">
-      <c r="A1046" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1046" t="n">
+      <c r="B2" t="n">
         <v>0.67</v>
       </c>
-      <c r="C1046" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1046" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1047">
-      <c r="A1047" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Mr. P</t>
         </is>
       </c>
-      <c r="B1047" t="n">
+      <c r="B3" t="n">
         <v>0.65</v>
       </c>
-      <c r="C1047" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1047" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1048">
-      <c r="A1048" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1048" t="n">
+      <c r="B4" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1048" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1048" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1049">
-      <c r="A1049" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Lou</t>
         </is>
       </c>
-      <c r="B1049" t="n">
+      <c r="B5" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1049" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1049" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1050">
-      <c r="A1050" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>8-Bit</t>
         </is>
       </c>
-      <c r="B1050" t="n">
+      <c r="B6" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1050" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1050" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1051">
-      <c r="A1051" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Colonel Ruffs</t>
         </is>
       </c>
-      <c r="B1051" t="n">
+      <c r="B7" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1051" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1051" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1052">
-      <c r="A1052" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Darryl</t>
         </is>
       </c>
-      <c r="B1052" t="n">
+      <c r="B8" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1052" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1052" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1053">
-      <c r="A1053" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Stu</t>
         </is>
       </c>
-      <c r="B1053" t="n">
+      <c r="B9" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1053" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1053" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1054">
-      <c r="A1054" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Sprout</t>
         </is>
       </c>
-      <c r="B1054" t="n">
+      <c r="B10" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1054" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1054" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1055">
-      <c r="A1055" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Byron</t>
         </is>
       </c>
-      <c r="B1055" t="n">
+      <c r="B11" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1055" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Dry Season</t>
         </is>
       </c>
-      <c r="D1055" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1056">
-      <c r="A1056" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Nani</t>
         </is>
       </c>
-      <c r="B1056" t="n">
+      <c r="B12" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1056" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1056" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1057">
-      <c r="A1057" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Darryl</t>
         </is>
       </c>
-      <c r="B1057" t="n">
+      <c r="B13" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1057" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1057" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1058">
-      <c r="A1058" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Colonel Ruffs</t>
         </is>
       </c>
-      <c r="B1058" t="n">
+      <c r="B14" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1058" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1058" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1059">
-      <c r="A1059" t="inlineStr">
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1059" t="n">
+      <c r="B15" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1059" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1059" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1060">
-      <c r="A1060" t="inlineStr">
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Mr. P</t>
         </is>
       </c>
-      <c r="B1060" t="n">
+      <c r="B16" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1060" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1060" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1061">
-      <c r="A1061" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Sprout</t>
         </is>
       </c>
-      <c r="B1061" t="n">
+      <c r="B17" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1061" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1061" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1062">
-      <c r="A1062" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1062" t="n">
+      <c r="B18" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1062" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1062" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1063">
-      <c r="A1063" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Poco</t>
         </is>
       </c>
-      <c r="B1063" t="n">
+      <c r="B19" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1063" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1063" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1064">
-      <c r="A1064" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Penny</t>
         </is>
       </c>
-      <c r="B1064" t="n">
+      <c r="B20" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1064" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1064" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1065">
-      <c r="A1065" t="inlineStr">
+    <row r="21">
+      <c r="A21" t="inlineStr">
         <is>
           <t>Tick</t>
         </is>
       </c>
-      <c r="B1065" t="n">
+      <c r="B21" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1065" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>Shooting Star</t>
         </is>
       </c>
-      <c r="D1065" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1066">
-      <c r="A1066" t="inlineStr">
+    <row r="22">
+      <c r="A22" t="inlineStr">
         <is>
           <t>Mr. P</t>
         </is>
       </c>
-      <c r="B1066" t="n">
+      <c r="B22" t="n">
         <v>0.65</v>
       </c>
-      <c r="C1066" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1066" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1067">
-      <c r="A1067" t="inlineStr">
+    <row r="23">
+      <c r="A23" t="inlineStr">
         <is>
           <t>Colonel Ruffs</t>
         </is>
       </c>
-      <c r="B1067" t="n">
+      <c r="B23" t="n">
         <v>0.65</v>
       </c>
-      <c r="C1067" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1067" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1068">
-      <c r="A1068" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1068" t="n">
+      <c r="B24" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1068" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1068" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1069">
-      <c r="A1069" t="inlineStr">
+    <row r="25">
+      <c r="A25" t="inlineStr">
         <is>
           <t>Jacky</t>
         </is>
       </c>
-      <c r="B1069" t="n">
+      <c r="B25" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1069" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1069" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1070">
-      <c r="A1070" t="inlineStr">
+    <row r="26">
+      <c r="A26" t="inlineStr">
         <is>
           <t>Gene</t>
         </is>
       </c>
-      <c r="B1070" t="n">
+      <c r="B26" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1070" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1070" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1071">
-      <c r="A1071" t="inlineStr">
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Poco</t>
         </is>
       </c>
-      <c r="B1071" t="n">
+      <c r="B27" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1071" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1071" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1072">
-      <c r="A1072" t="inlineStr">
+    <row r="28">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Rosa</t>
         </is>
       </c>
-      <c r="B1072" t="n">
+      <c r="B28" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1072" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1072" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1073">
-      <c r="A1073" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
         <is>
           <t>Penny</t>
         </is>
       </c>
-      <c r="B1073" t="n">
+      <c r="B29" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1073" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1073" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1074">
-      <c r="A1074" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1074" t="n">
+      <c r="B30" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1074" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1074" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1075">
-      <c r="A1075" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Brock</t>
         </is>
       </c>
-      <c r="B1075" t="n">
+      <c r="B31" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1075" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>Canal Grande</t>
         </is>
       </c>
-      <c r="D1075" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>Bounty</t>
         </is>
       </c>
     </row>
-    <row r="1076">
-      <c r="A1076" t="inlineStr">
+    <row r="32">
+      <c r="A32" t="inlineStr">
         <is>
           <t>Jacky</t>
         </is>
       </c>
-      <c r="B1076" t="n">
+      <c r="B32" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1076" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1076" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1077">
-      <c r="A1077" t="inlineStr">
+    <row r="33">
+      <c r="A33" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1077" t="n">
+      <c r="B33" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1077" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1077" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1078">
-      <c r="A1078" t="inlineStr">
+    <row r="34">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Nita</t>
         </is>
       </c>
-      <c r="B1078" t="n">
+      <c r="B34" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1078" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1078" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1079">
-      <c r="A1079" t="inlineStr">
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>Rosa</t>
         </is>
       </c>
-      <c r="B1079" t="n">
+      <c r="B35" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1079" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1079" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1080">
-      <c r="A1080" t="inlineStr">
+    <row r="36">
+      <c r="A36" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1080" t="n">
+      <c r="B36" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1080" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1080" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1081">
-      <c r="A1081" t="inlineStr">
+    <row r="37">
+      <c r="A37" t="inlineStr">
         <is>
           <t>Jessie</t>
         </is>
       </c>
-      <c r="B1081" t="n">
+      <c r="B37" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1081" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1081" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1082">
-      <c r="A1082" t="inlineStr">
+    <row r="38">
+      <c r="A38" t="inlineStr">
         <is>
           <t>Sandy</t>
         </is>
       </c>
-      <c r="B1082" t="n">
+      <c r="B38" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1082" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1082" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1083">
-      <c r="A1083" t="inlineStr">
+    <row r="39">
+      <c r="A39" t="inlineStr">
         <is>
           <t>Emz</t>
         </is>
       </c>
-      <c r="B1083" t="n">
+      <c r="B39" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1083" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1083" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1084">
-      <c r="A1084" t="inlineStr">
+    <row r="40">
+      <c r="A40" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="B1084" t="n">
+      <c r="B40" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1084" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1084" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1085">
-      <c r="A1085" t="inlineStr">
+    <row r="41">
+      <c r="A41" t="inlineStr">
         <is>
           <t>Frank</t>
         </is>
       </c>
-      <c r="B1085" t="n">
+      <c r="B41" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1085" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>Super Stadium</t>
         </is>
       </c>
-      <c r="D1085" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1086">
-      <c r="A1086" t="inlineStr">
+    <row r="42">
+      <c r="A42" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1086" t="n">
+      <c r="B42" t="n">
         <v>0.65</v>
       </c>
-      <c r="C1086" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1086" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1087">
-      <c r="A1087" t="inlineStr">
+    <row r="43">
+      <c r="A43" t="inlineStr">
         <is>
           <t>Pam</t>
         </is>
       </c>
-      <c r="B1087" t="n">
+      <c r="B43" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1087" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1087" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1088">
-      <c r="A1088" t="inlineStr">
+    <row r="44">
+      <c r="A44" t="inlineStr">
         <is>
           <t>Amber</t>
         </is>
       </c>
-      <c r="B1088" t="n">
+      <c r="B44" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1088" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1088" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1089">
-      <c r="A1089" t="inlineStr">
+    <row r="45">
+      <c r="A45" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1089" t="n">
+      <c r="B45" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1089" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1089" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1090">
-      <c r="A1090" t="inlineStr">
+    <row r="46">
+      <c r="A46" t="inlineStr">
         <is>
           <t>Lou</t>
         </is>
       </c>
-      <c r="B1090" t="n">
+      <c r="B46" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1090" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1090" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1091">
-      <c r="A1091" t="inlineStr">
+    <row r="47">
+      <c r="A47" t="inlineStr">
         <is>
           <t>Gale</t>
         </is>
       </c>
-      <c r="B1091" t="n">
+      <c r="B47" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1091" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1091" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1092">
-      <c r="A1092" t="inlineStr">
+    <row r="48">
+      <c r="A48" t="inlineStr">
         <is>
           <t>Frank</t>
         </is>
       </c>
-      <c r="B1092" t="n">
+      <c r="B48" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1092" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1092" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1093">
-      <c r="A1093" t="inlineStr">
+    <row r="49">
+      <c r="A49" t="inlineStr">
         <is>
           <t>8-Bit</t>
         </is>
       </c>
-      <c r="B1093" t="n">
+      <c r="B49" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1093" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1093" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1094">
-      <c r="A1094" t="inlineStr">
+    <row r="50">
+      <c r="A50" t="inlineStr">
         <is>
           <t>Poco</t>
         </is>
       </c>
-      <c r="B1094" t="n">
+      <c r="B50" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1094" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1094" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1095">
-      <c r="A1095" t="inlineStr">
+    <row r="51">
+      <c r="A51" t="inlineStr">
         <is>
           <t>Crow</t>
         </is>
       </c>
-      <c r="B1095" t="n">
+      <c r="B51" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1095" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>Backyard Bowl</t>
         </is>
       </c>
-      <c r="D1095" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>Brawl Ball</t>
         </is>
       </c>
     </row>
-    <row r="1096">
-      <c r="A1096" t="inlineStr">
+    <row r="52">
+      <c r="A52" t="inlineStr">
         <is>
           <t>Nita</t>
         </is>
       </c>
-      <c r="B1096" t="n">
+      <c r="B52" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1096" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1096" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1097">
-      <c r="A1097" t="inlineStr">
+    <row r="53">
+      <c r="A53" t="inlineStr">
         <is>
           <t>Jessie</t>
         </is>
       </c>
-      <c r="B1097" t="n">
+      <c r="B53" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1097" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1097" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1098">
-      <c r="A1098" t="inlineStr">
+    <row r="54">
+      <c r="A54" t="inlineStr">
         <is>
           <t>Amber</t>
         </is>
       </c>
-      <c r="B1098" t="n">
+      <c r="B54" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1098" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1098" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1099">
-      <c r="A1099" t="inlineStr">
+    <row r="55">
+      <c r="A55" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="B1099" t="n">
+      <c r="B55" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1099" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1099" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1100">
-      <c r="A1100" t="inlineStr">
+    <row r="56">
+      <c r="A56" t="inlineStr">
         <is>
           <t>Penny</t>
         </is>
       </c>
-      <c r="B1100" t="n">
+      <c r="B56" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1100" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1100" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1101">
-      <c r="A1101" t="inlineStr">
+    <row r="57">
+      <c r="A57" t="inlineStr">
         <is>
           <t>Sandy</t>
         </is>
       </c>
-      <c r="B1101" t="n">
+      <c r="B57" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1101" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1101" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1102">
-      <c r="A1102" t="inlineStr">
+    <row r="58">
+      <c r="A58" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1102" t="n">
+      <c r="B58" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1102" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1102" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1103">
-      <c r="A1103" t="inlineStr">
+    <row r="59">
+      <c r="A59" t="inlineStr">
         <is>
           <t>Darryl</t>
         </is>
       </c>
-      <c r="B1103" t="n">
+      <c r="B59" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1103" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1103" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1104">
-      <c r="A1104" t="inlineStr">
+    <row r="60">
+      <c r="A60" t="inlineStr">
         <is>
           <t>Crow</t>
         </is>
       </c>
-      <c r="B1104" t="n">
+      <c r="B60" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1104" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1104" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1105">
-      <c r="A1105" t="inlineStr">
+    <row r="61">
+      <c r="A61" t="inlineStr">
         <is>
           <t>Pam</t>
         </is>
       </c>
-      <c r="B1105" t="n">
+      <c r="B61" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1105" t="inlineStr">
+      <c r="C61" t="inlineStr">
         <is>
           <t>Double Swoosh</t>
         </is>
       </c>
-      <c r="D1105" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1106">
-      <c r="A1106" t="inlineStr">
+    <row r="62">
+      <c r="A62" t="inlineStr">
         <is>
           <t>Nita</t>
         </is>
       </c>
-      <c r="B1106" t="n">
+      <c r="B62" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1106" t="inlineStr">
+      <c r="C62" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1106" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1107">
-      <c r="A1107" t="inlineStr">
+    <row r="63">
+      <c r="A63" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1107" t="n">
+      <c r="B63" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1107" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1107" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1108">
-      <c r="A1108" t="inlineStr">
+    <row r="64">
+      <c r="A64" t="inlineStr">
         <is>
           <t>Colonel Ruffs</t>
         </is>
       </c>
-      <c r="B1108" t="n">
+      <c r="B64" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1108" t="inlineStr">
+      <c r="C64" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1108" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1109">
-      <c r="A1109" t="inlineStr">
+    <row r="65">
+      <c r="A65" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1109" t="n">
+      <c r="B65" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1109" t="inlineStr">
+      <c r="C65" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1109" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1110">
-      <c r="A1110" t="inlineStr">
+    <row r="66">
+      <c r="A66" t="inlineStr">
         <is>
           <t>Rosa</t>
         </is>
       </c>
-      <c r="B1110" t="n">
+      <c r="B66" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1110" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1110" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1111">
-      <c r="A1111" t="inlineStr">
+    <row r="67">
+      <c r="A67" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="B1111" t="n">
+      <c r="B67" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1111" t="inlineStr">
+      <c r="C67" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1111" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1112">
-      <c r="A1112" t="inlineStr">
+    <row r="68">
+      <c r="A68" t="inlineStr">
         <is>
           <t>8-Bit</t>
         </is>
       </c>
-      <c r="B1112" t="n">
+      <c r="B68" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1112" t="inlineStr">
+      <c r="C68" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1112" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1113">
-      <c r="A1113" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
         <is>
           <t>Penny</t>
         </is>
       </c>
-      <c r="B1113" t="n">
+      <c r="B69" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1113" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1113" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1114">
-      <c r="A1114" t="inlineStr">
+    <row r="70">
+      <c r="A70" t="inlineStr">
         <is>
           <t>Sandy</t>
         </is>
       </c>
-      <c r="B1114" t="n">
+      <c r="B70" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1114" t="inlineStr">
+      <c r="C70" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1114" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1115">
-      <c r="A1115" t="inlineStr">
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>Darryl</t>
         </is>
       </c>
-      <c r="B1115" t="n">
+      <c r="B71" t="n">
         <v>0.58</v>
       </c>
-      <c r="C1115" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>Hard Rock Mine</t>
         </is>
       </c>
-      <c r="D1115" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1116">
-      <c r="A1116" t="inlineStr">
+    <row r="72">
+      <c r="A72" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1116" t="n">
+      <c r="B72" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1116" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1116" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1117">
-      <c r="A1117" t="inlineStr">
+    <row r="73">
+      <c r="A73" t="inlineStr">
         <is>
           <t>Sandy</t>
         </is>
       </c>
-      <c r="B1117" t="n">
+      <c r="B73" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1117" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1117" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1118">
-      <c r="A1118" t="inlineStr">
+    <row r="74">
+      <c r="A74" t="inlineStr">
         <is>
           <t>Crow</t>
         </is>
       </c>
-      <c r="B1118" t="n">
+      <c r="B74" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1118" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1118" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1119">
-      <c r="A1119" t="inlineStr">
+    <row r="75">
+      <c r="A75" t="inlineStr">
         <is>
           <t>Nita</t>
         </is>
       </c>
-      <c r="B1119" t="n">
+      <c r="B75" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1119" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1119" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1120">
-      <c r="A1120" t="inlineStr">
+    <row r="76">
+      <c r="A76" t="inlineStr">
         <is>
           <t>Jessie</t>
         </is>
       </c>
-      <c r="B1120" t="n">
+      <c r="B76" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1120" t="inlineStr">
+      <c r="C76" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1120" t="inlineStr">
+      <c r="D76" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1121">
-      <c r="A1121" t="inlineStr">
+    <row r="77">
+      <c r="A77" t="inlineStr">
         <is>
           <t>Darryl</t>
         </is>
       </c>
-      <c r="B1121" t="n">
+      <c r="B77" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1121" t="inlineStr">
+      <c r="C77" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1121" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1122">
-      <c r="A1122" t="inlineStr">
+    <row r="78">
+      <c r="A78" t="inlineStr">
         <is>
           <t>El Primo</t>
         </is>
       </c>
-      <c r="B1122" t="n">
+      <c r="B78" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1122" t="inlineStr">
+      <c r="C78" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1122" t="inlineStr">
+      <c r="D78" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1123">
-      <c r="A1123" t="inlineStr">
+    <row r="79">
+      <c r="A79" t="inlineStr">
         <is>
           <t>Penny</t>
         </is>
       </c>
-      <c r="B1123" t="n">
+      <c r="B79" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1123" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1123" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1124">
-      <c r="A1124" t="inlineStr">
+    <row r="80">
+      <c r="A80" t="inlineStr">
         <is>
           <t>Lou</t>
         </is>
       </c>
-      <c r="B1124" t="n">
+      <c r="B80" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1124" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1124" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1125">
-      <c r="A1125" t="inlineStr">
+    <row r="81">
+      <c r="A81" t="inlineStr">
         <is>
           <t>Stu</t>
         </is>
       </c>
-      <c r="B1125" t="n">
+      <c r="B81" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1125" t="inlineStr">
+      <c r="C81" t="inlineStr">
         <is>
           <t>Minecart Madness</t>
         </is>
       </c>
-      <c r="D1125" t="inlineStr">
+      <c r="D81" t="inlineStr">
         <is>
           <t>Gem Grab</t>
         </is>
       </c>
     </row>
-    <row r="1126">
-      <c r="A1126" t="inlineStr">
+    <row r="82">
+      <c r="A82" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1126" t="n">
+      <c r="B82" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="C1126" t="inlineStr">
+      <c r="C82" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1126" t="inlineStr">
+      <c r="D82" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1127">
-      <c r="A1127" t="inlineStr">
+    <row r="83">
+      <c r="A83" t="inlineStr">
         <is>
           <t>Bea</t>
         </is>
       </c>
-      <c r="B1127" t="n">
+      <c r="B83" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1127" t="inlineStr">
+      <c r="C83" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1127" t="inlineStr">
+      <c r="D83" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1128">
-      <c r="A1128" t="inlineStr">
+    <row r="84">
+      <c r="A84" t="inlineStr">
         <is>
           <t>Pam</t>
         </is>
       </c>
-      <c r="B1128" t="n">
+      <c r="B84" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1128" t="inlineStr">
+      <c r="C84" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1128" t="inlineStr">
+      <c r="D84" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1129">
-      <c r="A1129" t="inlineStr">
+    <row r="85">
+      <c r="A85" t="inlineStr">
         <is>
           <t>Nita</t>
         </is>
       </c>
-      <c r="B1129" t="n">
+      <c r="B85" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1129" t="inlineStr">
+      <c r="C85" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1129" t="inlineStr">
+      <c r="D85" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1130">
-      <c r="A1130" t="inlineStr">
+    <row r="86">
+      <c r="A86" t="inlineStr">
         <is>
           <t>Bull</t>
         </is>
       </c>
-      <c r="B1130" t="n">
+      <c r="B86" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1130" t="inlineStr">
+      <c r="C86" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1130" t="inlineStr">
+      <c r="D86" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1131">
-      <c r="A1131" t="inlineStr">
+    <row r="87">
+      <c r="A87" t="inlineStr">
         <is>
           <t>Emz</t>
         </is>
       </c>
-      <c r="B1131" t="n">
+      <c r="B87" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1131" t="inlineStr">
+      <c r="C87" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1131" t="inlineStr">
+      <c r="D87" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1132">
-      <c r="A1132" t="inlineStr">
+    <row r="88">
+      <c r="A88" t="inlineStr">
         <is>
           <t>Colette</t>
         </is>
       </c>
-      <c r="B1132" t="n">
+      <c r="B88" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1132" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1132" t="inlineStr">
+      <c r="D88" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1133">
-      <c r="A1133" t="inlineStr">
+    <row r="89">
+      <c r="A89" t="inlineStr">
         <is>
           <t>Jessie</t>
         </is>
       </c>
-      <c r="B1133" t="n">
+      <c r="B89" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1133" t="inlineStr">
+      <c r="C89" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1133" t="inlineStr">
+      <c r="D89" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1134">
-      <c r="A1134" t="inlineStr">
+    <row r="90">
+      <c r="A90" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1134" t="n">
+      <c r="B90" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1134" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1134" t="inlineStr">
+      <c r="D90" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1135">
-      <c r="A1135" t="inlineStr">
+    <row r="91">
+      <c r="A91" t="inlineStr">
         <is>
           <t>Edgar</t>
         </is>
       </c>
-      <c r="B1135" t="n">
+      <c r="B91" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1135" t="inlineStr">
+      <c r="C91" t="inlineStr">
         <is>
           <t>Safe Zone</t>
         </is>
       </c>
-      <c r="D1135" t="inlineStr">
+      <c r="D91" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1136">
-      <c r="A1136" t="inlineStr">
+    <row r="92">
+      <c r="A92" t="inlineStr">
         <is>
           <t>Nita</t>
         </is>
       </c>
-      <c r="B1136" t="n">
+      <c r="B92" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1136" t="inlineStr">
+      <c r="C92" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1136" t="inlineStr">
+      <c r="D92" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1137">
-      <c r="A1137" t="inlineStr">
+    <row r="93">
+      <c r="A93" t="inlineStr">
         <is>
           <t>Bibi</t>
         </is>
       </c>
-      <c r="B1137" t="n">
+      <c r="B93" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1137" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1137" t="inlineStr">
+      <c r="D93" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1138">
-      <c r="A1138" t="inlineStr">
+    <row r="94">
+      <c r="A94" t="inlineStr">
         <is>
           <t>Darryl</t>
         </is>
       </c>
-      <c r="B1138" t="n">
+      <c r="B94" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1138" t="inlineStr">
+      <c r="C94" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1138" t="inlineStr">
+      <c r="D94" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1139">
-      <c r="A1139" t="inlineStr">
+    <row r="95">
+      <c r="A95" t="inlineStr">
         <is>
           <t>Rosa</t>
         </is>
       </c>
-      <c r="B1139" t="n">
+      <c r="B95" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1139" t="inlineStr">
+      <c r="C95" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1139" t="inlineStr">
+      <c r="D95" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1140">
-      <c r="A1140" t="inlineStr">
+    <row r="96">
+      <c r="A96" t="inlineStr">
         <is>
           <t>El Primo</t>
         </is>
       </c>
-      <c r="B1140" t="n">
+      <c r="B96" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1140" t="inlineStr">
+      <c r="C96" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1140" t="inlineStr">
+      <c r="D96" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1141">
-      <c r="A1141" t="inlineStr">
+    <row r="97">
+      <c r="A97" t="inlineStr">
         <is>
           <t>Edgar</t>
         </is>
       </c>
-      <c r="B1141" t="n">
+      <c r="B97" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1141" t="inlineStr">
+      <c r="C97" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1141" t="inlineStr">
+      <c r="D97" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1142">
-      <c r="A1142" t="inlineStr">
+    <row r="98">
+      <c r="A98" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="B1142" t="n">
+      <c r="B98" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1142" t="inlineStr">
+      <c r="C98" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1142" t="inlineStr">
+      <c r="D98" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1143">
-      <c r="A1143" t="inlineStr">
+    <row r="99">
+      <c r="A99" t="inlineStr">
         <is>
           <t>Stu</t>
         </is>
       </c>
-      <c r="B1143" t="n">
+      <c r="B99" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1143" t="inlineStr">
+      <c r="C99" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1143" t="inlineStr">
+      <c r="D99" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1144">
-      <c r="A1144" t="inlineStr">
+    <row r="100">
+      <c r="A100" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1144" t="n">
+      <c r="B100" t="n">
         <v>0.58</v>
       </c>
-      <c r="C1144" t="inlineStr">
+      <c r="C100" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1144" t="inlineStr">
+      <c r="D100" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1145">
-      <c r="A1145" t="inlineStr">
+    <row r="101">
+      <c r="A101" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1145" t="n">
+      <c r="B101" t="n">
         <v>0.58</v>
       </c>
-      <c r="C1145" t="inlineStr">
+      <c r="C101" t="inlineStr">
         <is>
           <t>Hot Potato</t>
         </is>
       </c>
-      <c r="D1145" t="inlineStr">
+      <c r="D101" t="inlineStr">
         <is>
           <t>Heist</t>
         </is>
       </c>
     </row>
-    <row r="1146">
-      <c r="A1146" t="inlineStr">
+    <row r="102">
+      <c r="A102" t="inlineStr">
         <is>
           <t>Amber</t>
         </is>
       </c>
-      <c r="B1146" t="n">
+      <c r="B102" t="n">
         <v>0.66</v>
       </c>
-      <c r="C1146" t="inlineStr">
+      <c r="C102" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1146" t="inlineStr">
+      <c r="D102" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1147">
-      <c r="A1147" t="inlineStr">
+    <row r="103">
+      <c r="A103" t="inlineStr">
         <is>
           <t>Bea</t>
         </is>
       </c>
-      <c r="B1147" t="n">
+      <c r="B103" t="n">
         <v>0.66</v>
       </c>
-      <c r="C1147" t="inlineStr">
+      <c r="C103" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1147" t="inlineStr">
+      <c r="D103" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1148">
-      <c r="A1148" t="inlineStr">
+    <row r="104">
+      <c r="A104" t="inlineStr">
         <is>
           <t>Emz</t>
         </is>
       </c>
-      <c r="B1148" t="n">
+      <c r="B104" t="n">
         <v>0.65</v>
       </c>
-      <c r="C1148" t="inlineStr">
+      <c r="C104" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1148" t="inlineStr">
+      <c r="D104" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1149">
-      <c r="A1149" t="inlineStr">
+    <row r="105">
+      <c r="A105" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1149" t="n">
+      <c r="B105" t="n">
         <v>0.65</v>
       </c>
-      <c r="C1149" t="inlineStr">
+      <c r="C105" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1149" t="inlineStr">
+      <c r="D105" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1150">
-      <c r="A1150" t="inlineStr">
+    <row r="106">
+      <c r="A106" t="inlineStr">
         <is>
           <t>Lou</t>
         </is>
       </c>
-      <c r="B1150" t="n">
+      <c r="B106" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1150" t="inlineStr">
+      <c r="C106" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1150" t="inlineStr">
+      <c r="D106" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1151">
-      <c r="A1151" t="inlineStr">
+    <row r="107">
+      <c r="A107" t="inlineStr">
         <is>
           <t>Sandy</t>
         </is>
       </c>
-      <c r="B1151" t="n">
+      <c r="B107" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1151" t="inlineStr">
+      <c r="C107" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1151" t="inlineStr">
+      <c r="D107" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1152">
-      <c r="A1152" t="inlineStr">
+    <row r="108">
+      <c r="A108" t="inlineStr">
         <is>
           <t>Gale</t>
         </is>
       </c>
-      <c r="B1152" t="n">
+      <c r="B108" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1152" t="inlineStr">
+      <c r="C108" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1152" t="inlineStr">
+      <c r="D108" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1153">
-      <c r="A1153" t="inlineStr">
+    <row r="109">
+      <c r="A109" t="inlineStr">
         <is>
           <t>El Primo</t>
         </is>
       </c>
-      <c r="B1153" t="n">
+      <c r="B109" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1153" t="inlineStr">
+      <c r="C109" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1153" t="inlineStr">
+      <c r="D109" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1154">
-      <c r="A1154" t="inlineStr">
+    <row r="110">
+      <c r="A110" t="inlineStr">
         <is>
           <t>Poco</t>
         </is>
       </c>
-      <c r="B1154" t="n">
+      <c r="B110" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1154" t="inlineStr">
+      <c r="C110" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1154" t="inlineStr">
+      <c r="D110" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1155">
-      <c r="A1155" t="inlineStr">
+    <row r="111">
+      <c r="A111" t="inlineStr">
         <is>
           <t>8-Bit</t>
         </is>
       </c>
-      <c r="B1155" t="n">
+      <c r="B111" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1155" t="inlineStr">
+      <c r="C111" t="inlineStr">
         <is>
           <t>Ring of Fire</t>
         </is>
       </c>
-      <c r="D1155" t="inlineStr">
+      <c r="D111" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1156">
-      <c r="A1156" t="inlineStr">
+    <row r="112">
+      <c r="A112" t="inlineStr">
         <is>
           <t>Frank</t>
         </is>
       </c>
-      <c r="B1156" t="n">
+      <c r="B112" t="n">
         <v>0.65</v>
       </c>
-      <c r="C1156" t="inlineStr">
+      <c r="C112" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1156" t="inlineStr">
+      <c r="D112" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1157">
-      <c r="A1157" t="inlineStr">
+    <row r="113">
+      <c r="A113" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1157" t="n">
+      <c r="B113" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1157" t="inlineStr">
+      <c r="C113" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1157" t="inlineStr">
+      <c r="D113" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1158">
-      <c r="A1158" t="inlineStr">
+    <row r="114">
+      <c r="A114" t="inlineStr">
         <is>
           <t>Nita</t>
         </is>
       </c>
-      <c r="B1158" t="n">
+      <c r="B114" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1158" t="inlineStr">
+      <c r="C114" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1158" t="inlineStr">
+      <c r="D114" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1159">
-      <c r="A1159" t="inlineStr">
+    <row r="115">
+      <c r="A115" t="inlineStr">
         <is>
           <t>Rosa</t>
         </is>
       </c>
-      <c r="B1159" t="n">
+      <c r="B115" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1159" t="inlineStr">
+      <c r="C115" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1159" t="inlineStr">
+      <c r="D115" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1160">
-      <c r="A1160" t="inlineStr">
+    <row r="116">
+      <c r="A116" t="inlineStr">
         <is>
           <t>Colette</t>
         </is>
       </c>
-      <c r="B1160" t="n">
+      <c r="B116" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1160" t="inlineStr">
+      <c r="C116" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1160" t="inlineStr">
+      <c r="D116" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1161">
-      <c r="A1161" t="inlineStr">
+    <row r="117">
+      <c r="A117" t="inlineStr">
         <is>
           <t>Gale</t>
         </is>
       </c>
-      <c r="B1161" t="n">
+      <c r="B117" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1161" t="inlineStr">
+      <c r="C117" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1161" t="inlineStr">
+      <c r="D117" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1162">
-      <c r="A1162" t="inlineStr">
+    <row r="118">
+      <c r="A118" t="inlineStr">
         <is>
           <t>Darryl</t>
         </is>
       </c>
-      <c r="B1162" t="n">
+      <c r="B118" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1162" t="inlineStr">
+      <c r="C118" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1162" t="inlineStr">
+      <c r="D118" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1163">
-      <c r="A1163" t="inlineStr">
+    <row r="119">
+      <c r="A119" t="inlineStr">
         <is>
           <t>Lou</t>
         </is>
       </c>
-      <c r="B1163" t="n">
+      <c r="B119" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1163" t="inlineStr">
+      <c r="C119" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1163" t="inlineStr">
+      <c r="D119" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1164">
-      <c r="A1164" t="inlineStr">
+    <row r="120">
+      <c r="A120" t="inlineStr">
         <is>
           <t>Bibi</t>
         </is>
       </c>
-      <c r="B1164" t="n">
+      <c r="B120" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1164" t="inlineStr">
+      <c r="C120" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1164" t="inlineStr">
+      <c r="D120" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1165">
-      <c r="A1165" t="inlineStr">
+    <row r="121">
+      <c r="A121" t="inlineStr">
         <is>
           <t>Jacky</t>
         </is>
       </c>
-      <c r="B1165" t="n">
+      <c r="B121" t="n">
         <v>0.59</v>
       </c>
-      <c r="C1165" t="inlineStr">
+      <c r="C121" t="inlineStr">
         <is>
           <t>Split</t>
         </is>
       </c>
-      <c r="D1165" t="inlineStr">
+      <c r="D121" t="inlineStr">
         <is>
           <t>Hot Zone</t>
         </is>
       </c>
     </row>
-    <row r="1166">
-      <c r="A1166" t="inlineStr">
+    <row r="122">
+      <c r="A122" t="inlineStr">
         <is>
           <t>Frank</t>
         </is>
       </c>
-      <c r="B1166" t="n">
+      <c r="B122" t="n">
         <v>0.67</v>
       </c>
-      <c r="C1166" t="inlineStr">
+      <c r="C122" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1166" t="inlineStr">
+      <c r="D122" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1167">
-      <c r="A1167" t="inlineStr">
+    <row r="123">
+      <c r="A123" t="inlineStr">
         <is>
           <t>Belle</t>
         </is>
       </c>
-      <c r="B1167" t="n">
+      <c r="B123" t="n">
         <v>0.66</v>
       </c>
-      <c r="C1167" t="inlineStr">
+      <c r="C123" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1167" t="inlineStr">
+      <c r="D123" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1168">
-      <c r="A1168" t="inlineStr">
+    <row r="124">
+      <c r="A124" t="inlineStr">
         <is>
           <t>Carl</t>
         </is>
       </c>
-      <c r="B1168" t="n">
+      <c r="B124" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1168" t="inlineStr">
+      <c r="C124" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1168" t="inlineStr">
+      <c r="D124" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1169">
-      <c r="A1169" t="inlineStr">
+    <row r="125">
+      <c r="A125" t="inlineStr">
         <is>
           <t>Lou</t>
         </is>
       </c>
-      <c r="B1169" t="n">
+      <c r="B125" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1169" t="inlineStr">
+      <c r="C125" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1169" t="inlineStr">
+      <c r="D125" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1170">
-      <c r="A1170" t="inlineStr">
+    <row r="126">
+      <c r="A126" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1170" t="n">
+      <c r="B126" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1170" t="inlineStr">
+      <c r="C126" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1170" t="inlineStr">
+      <c r="D126" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1171">
-      <c r="A1171" t="inlineStr">
+    <row r="127">
+      <c r="A127" t="inlineStr">
         <is>
           <t>Amber</t>
         </is>
       </c>
-      <c r="B1171" t="n">
+      <c r="B127" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1171" t="inlineStr">
+      <c r="C127" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1171" t="inlineStr">
+      <c r="D127" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1172">
-      <c r="A1172" t="inlineStr">
+    <row r="128">
+      <c r="A128" t="inlineStr">
         <is>
           <t>Barley</t>
         </is>
       </c>
-      <c r="B1172" t="n">
+      <c r="B128" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1172" t="inlineStr">
+      <c r="C128" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1172" t="inlineStr">
+      <c r="D128" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1173">
-      <c r="A1173" t="inlineStr">
+    <row r="129">
+      <c r="A129" t="inlineStr">
         <is>
           <t>Crow</t>
         </is>
       </c>
-      <c r="B1173" t="n">
+      <c r="B129" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1173" t="inlineStr">
+      <c r="C129" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1173" t="inlineStr">
+      <c r="D129" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1174">
-      <c r="A1174" t="inlineStr">
+    <row r="130">
+      <c r="A130" t="inlineStr">
         <is>
           <t>Colonel Ruffs</t>
         </is>
       </c>
-      <c r="B1174" t="n">
+      <c r="B130" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1174" t="inlineStr">
+      <c r="C130" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1174" t="inlineStr">
+      <c r="D130" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1175">
-      <c r="A1175" t="inlineStr">
+    <row r="131">
+      <c r="A131" t="inlineStr">
         <is>
           <t>Stu</t>
         </is>
       </c>
-      <c r="B1175" t="n">
+      <c r="B131" t="n">
         <v>0.6</v>
       </c>
-      <c r="C1175" t="inlineStr">
+      <c r="C131" t="inlineStr">
         <is>
           <t>Factory Rush</t>
         </is>
       </c>
-      <c r="D1175" t="inlineStr">
+      <c r="D131" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1176">
-      <c r="A1176" t="inlineStr">
+    <row r="132">
+      <c r="A132" t="inlineStr">
         <is>
           <t>Lou</t>
         </is>
       </c>
-      <c r="B1176" t="n">
+      <c r="B132" t="n">
         <v>0.66</v>
       </c>
-      <c r="C1176" t="inlineStr">
+      <c r="C132" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1176" t="inlineStr">
+      <c r="D132" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1177">
-      <c r="A1177" t="inlineStr">
+    <row r="133">
+      <c r="A133" t="inlineStr">
         <is>
           <t>El Primo</t>
         </is>
       </c>
-      <c r="B1177" t="n">
+      <c r="B133" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1177" t="inlineStr">
+      <c r="C133" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1177" t="inlineStr">
+      <c r="D133" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1178">
-      <c r="A1178" t="inlineStr">
+    <row r="134">
+      <c r="A134" t="inlineStr">
         <is>
           <t>Dynamike</t>
         </is>
       </c>
-      <c r="B1178" t="n">
+      <c r="B134" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1178" t="inlineStr">
+      <c r="C134" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1178" t="inlineStr">
+      <c r="D134" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1179">
-      <c r="A1179" t="inlineStr">
+    <row r="135">
+      <c r="A135" t="inlineStr">
         <is>
           <t>Carl</t>
         </is>
       </c>
-      <c r="B1179" t="n">
+      <c r="B135" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1179" t="inlineStr">
+      <c r="C135" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1179" t="inlineStr">
+      <c r="D135" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1180">
-      <c r="A1180" t="inlineStr">
+    <row r="136">
+      <c r="A136" t="inlineStr">
         <is>
           <t>Bo</t>
         </is>
       </c>
-      <c r="B1180" t="n">
+      <c r="B136" t="n">
         <v>0.64</v>
       </c>
-      <c r="C1180" t="inlineStr">
+      <c r="C136" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1180" t="inlineStr">
+      <c r="D136" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1181">
-      <c r="A1181" t="inlineStr">
+    <row r="137">
+      <c r="A137" t="inlineStr">
         <is>
           <t>Colonel Ruffs</t>
         </is>
       </c>
-      <c r="B1181" t="n">
+      <c r="B137" t="n">
         <v>0.63</v>
       </c>
-      <c r="C1181" t="inlineStr">
+      <c r="C137" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1181" t="inlineStr">
+      <c r="D137" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1182">
-      <c r="A1182" t="inlineStr">
+    <row r="138">
+      <c r="A138" t="inlineStr">
         <is>
           <t>Squeak</t>
         </is>
       </c>
-      <c r="B1182" t="n">
+      <c r="B138" t="n">
         <v>0.62</v>
       </c>
-      <c r="C1182" t="inlineStr">
+      <c r="C138" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1182" t="inlineStr">
+      <c r="D138" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1183">
-      <c r="A1183" t="inlineStr">
+    <row r="139">
+      <c r="A139" t="inlineStr">
         <is>
           <t>Sandy</t>
         </is>
       </c>
-      <c r="B1183" t="n">
+      <c r="B139" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1183" t="inlineStr">
+      <c r="C139" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1183" t="inlineStr">
+      <c r="D139" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1184">
-      <c r="A1184" t="inlineStr">
+    <row r="140">
+      <c r="A140" t="inlineStr">
         <is>
           <t>Frank</t>
         </is>
       </c>
-      <c r="B1184" t="n">
+      <c r="B140" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1184" t="inlineStr">
+      <c r="C140" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1184" t="inlineStr">
+      <c r="D140" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
-    <row r="1185">
-      <c r="A1185" t="inlineStr">
+    <row r="141">
+      <c r="A141" t="inlineStr">
         <is>
           <t>Surge</t>
         </is>
       </c>
-      <c r="B1185" t="n">
+      <c r="B141" t="n">
         <v>0.61</v>
       </c>
-      <c r="C1185" t="inlineStr">
+      <c r="C141" t="inlineStr">
         <is>
           <t>Nuts &amp; Bolts</t>
         </is>
       </c>
-      <c r="D1185" t="inlineStr">
+      <c r="D141" t="inlineStr">
         <is>
           <t>Siege</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>